<commit_message>
The first commit on Mar. 29th, 2019
</commit_message>
<xml_diff>
--- a/Python_Library.xlsx
+++ b/Python_Library.xlsx
@@ -4,17 +4,23 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ctypes" sheetId="1" r:id="rId1"/>
+    <sheet name="Built-in Functions" sheetId="2" r:id="rId2"/>
+    <sheet name="openpyxl" sheetId="3" r:id="rId3"/>
+    <sheet name="html" sheetId="4" r:id="rId4"/>
+    <sheet name="CSS" sheetId="5" r:id="rId5"/>
+    <sheet name="JS" sheetId="6" r:id="rId6"/>
+    <sheet name="encoding" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="160">
   <si>
     <t>1. 加载动态链接库： ctypes导出两种对象,cdll和windll，可以用于加载动态链接库。windll库采用stdcall调用函数，stdcall用cdecl调用函数。 在windows中导入动态链接库时可以像访问类属性那样，采用windll.XXX的方式，Windows会自动添加“.dll”后缀。</t>
   </si>
@@ -295,9 +301,6 @@
     </r>
   </si>
   <si>
-    <t>11. 可以通过byref()传引用，或pointer()传参</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">&gt;&gt;&gt; i = c_int()
 &gt;&gt;&gt; f = c_float()
@@ -432,6 +435,385 @@
 1 2 3 4 5 6 7 8 9 10
 &gt;&gt;&gt;
 </t>
+  </si>
+  <si>
+    <t>14. 指针</t>
+  </si>
+  <si>
+    <t>指针实例可以通过调用pointer()函数获得，指针实例有一个contents属性返回所指向的对象， 但是contents返回的是一个和原指针指向地址内容相同的新对象，不是原来的对象</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;&gt; from ctypes import *
+&gt;&gt;&gt; i = c_int(42)
+&gt;&gt;&gt; pi = pointer(i)
+&gt;&gt;&gt; pi.contents
+c_long(42)
+&gt;&gt;&gt; pi.contents is i
+False
+&gt;&gt;&gt; pi.contents is pi.contents
+False
+&gt;&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t>给pointer的contents属性赋新的对象则会使指针指向新的对象地址：</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;&gt; i = c_int(99)
+&gt;&gt;&gt; pi.contents = i
+&gt;&gt;&gt; pi.contents
+c_long(99)
+&gt;&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t>指针也可以通过序号访问，向指针的序号赋值也可以改变指针指向的对象，例如：</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;&gt; pi[0]
+99
+&gt;&gt;&gt; print(i)
+c_long(99)
+&gt;&gt;&gt; pi[0] = 22
+&gt;&gt;&gt; print(i)
+c_long(22)
+&gt;&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t>也可以使用非零序号，但是必须非常小心，通常只有当收到C函数传来的指针，并且知道该指针指向一个数组时才会这么用</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;&gt; PI = POINTER(c_int)
+&gt;&gt;&gt; PI
+&lt;class 'ctypes.LP_c_long'&gt;
+&gt;&gt;&gt; PI(42)
+Traceback (most recent call last):
+  File "&lt;stdin&gt;", line 1, in &lt;module&gt;
+TypeError: expected c_long instead of int
+&gt;&gt;&gt; PI(c_int(42))
+&lt;ctypes.LP_c_long object at 0x...&gt;
+&gt;&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t>实际上，pointer()函数是通过POINTER()函数来实现的，POINTER函数接受任何ctypes类型，并且返回一个新指针类型，该指针类型用ctypes类型对象初始化则生成指针</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;&gt; null_ptr = POINTER(c_int)()
+&gt;&gt;&gt; print(bool(null_ptr))
+False
+&gt;&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t>若初始化对象为空则生成空指针，ctypes会自动检查空指针</t>
+  </si>
+  <si>
+    <t>11. 可以通过byref()传引用，或pointer()传指针</t>
+  </si>
+  <si>
+    <t>15. 类型转换</t>
+  </si>
+  <si>
+    <t>ctypes 通常情况下会进行类型检查，但是也有例外，例如，POINTER(c_int)类型可以接收c_int数组类型，甚至如果一个指针类型（如POINTER(c_int)）在函数argtypes中声明，一个该指针所指向的类型可以直接传给该函数，ctypes会自动使用byref()进行转换（感觉byref很像C语言中的取地址符&amp;）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;&gt; class Bar(Structure):
+...     _fields_ = [("count", c_int), ("values", POINTER(c_int))]
+...
+&gt;&gt;&gt; bar = Bar()
+&gt;&gt;&gt; bar.values = (c_int * 3)(1, 2, 3)
+&gt;&gt;&gt; bar.count = 3
+&gt;&gt;&gt; for i in range(bar.count):
+...     print(bar.values[i])
+...
+1
+2
+3
+&gt;&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t>POINTER类型页可以指向None，即空指针</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;&gt; bar.values = None
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;&gt; a = (c_byte * 4)()
+&gt;&gt;&gt; cast(a, POINTER(c_int))
+&lt;ctypes.LP_c_long object at ...&gt;
+&gt;&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;&gt; bar = Bar()
+&gt;&gt;&gt; bar.values = cast((c_byte * 4)(), POINTER(c_int))
+&gt;&gt;&gt; print(bar.values[0])
+0
+&gt;&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t>16. 类型前向引用</t>
+  </si>
+  <si>
+    <t>C语言中的前向引用一般如下：</t>
+  </si>
+  <si>
+    <t xml:space="preserve">struct cell; /* forward declaration */
+struct cell {
+    char *name;
+    struct cell *next;
+};
+</t>
+  </si>
+  <si>
+    <t>在Python中可以这样实现：</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;&gt; from ctypes import *
+&gt;&gt;&gt; class cell(Structure):
+...     pass
+...
+&gt;&gt;&gt; cell._fields_ = [("name", c_char_p),
+...                  ("next", POINTER(cell))]
+&gt;&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t>当需要进行类型转换时，可以使用cast()函数。该函数用于将一个ctypes指针强制转换成其他ctypes类型的指针，它接受两个参数，待转换ctypes指针和目标指针类型，返回第二个参数类型的指针，指向第一个参数的地址</t>
+  </si>
+  <si>
+    <t>16. 回调函数</t>
+  </si>
+  <si>
+    <t>可以通过CFUNCTYPE()和WINFUNCTYPE()生成函数类型</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;&gt; IntArray5 = c_int * 5
+&gt;&gt;&gt; ia = IntArray5(5, 1, 7, 33, 99)
+&gt;&gt;&gt; qsort = libc.qsort
+&gt;&gt;&gt; qsort.restype = None
+&gt;&gt;&gt; CMPFUNC = CFUNCTYPE(c_int, POINTER(c_int), POINTER(c_int))
+&gt;&gt;&gt; def py_cmp_func(a, b):
+...     print("py_cmp_func", a[0], b[0])
+...     return 0
+...
+&gt;&gt;&gt; cmp_func = CMPFUNC(py_cmp_func)
+&gt;&gt;&gt; qsort(ia, len(ia), sizeof(c_int), cmp_func)  
+py_cmp_func 5 1
+py_cmp_func 33 99
+py_cmp_func 7 33
+py_cmp_func 5 7
+py_cmp_func 1 7
+&gt;&gt;&gt;
+</t>
+  </si>
+  <si>
+    <t>1. all()</t>
+  </si>
+  <si>
+    <t>所有元素为真则返回真</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def all(iterable):
+    for element in iterable:
+        if not element:
+            return False
+    return True
+</t>
+  </si>
+  <si>
+    <t>2.  any()</t>
+  </si>
+  <si>
+    <t>任意元素为真则返回真</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def any(iterable):
+    for element in iterable:
+        if element:
+            return True
+    return False
+</t>
+  </si>
+  <si>
+    <t>3. bool(x)</t>
+  </si>
+  <si>
+    <t>若x为零，为None或为空，则返回false，否则返回true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. bytearray([source[, encoding[, errors]]]) 
+</t>
+  </si>
+  <si>
+    <t>生成字节数组，若参数为字符串，则必须同时指定encoding； 若为数字，则生成相应大小的数组， 数组内容可更改</t>
+  </si>
+  <si>
+    <t>5. bytes()</t>
+  </si>
+  <si>
+    <t>功能和bytearray相同，但是生成打数组内容不可变</t>
+  </si>
+  <si>
+    <t>6. callable()</t>
+  </si>
+  <si>
+    <t>对象是否可调用，true未必可调用，false一定不可调用</t>
+  </si>
+  <si>
+    <t>7. chr()</t>
+  </si>
+  <si>
+    <t>inverse of ord()</t>
+  </si>
+  <si>
+    <t>8. delattr(object, name)</t>
+  </si>
+  <si>
+    <t>setattr()对应的函数， 另外， 类中定义的__getattr__(self, item)函数和__getattribute__(self, item)函数的区别是，前者只有当item未在类中定义时才被调用，后者无论item是否存在都被调用，当获取对象属性时，后者先被调用，若产生AtrributeError异常，前者则被调用</t>
+  </si>
+  <si>
+    <t>9. divmod(a,b)</t>
+  </si>
+  <si>
+    <t>返回一个tuple， 分别是除数和余数</t>
+  </si>
+  <si>
+    <t>10. enumerate(iterable, start=0)</t>
+  </si>
+  <si>
+    <t>返回一个迭代器，该迭代器的元素由一个计数值和iterable的元素组成</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt;&gt; seasons = ['Spring', 'Summer', 'Fall', 'Winter']
+&gt;&gt;&gt; list(enumerate(seasons))
+[(0, 'Spring'), (1, 'Summer'), (2, 'Fall'), (3, 'Winter')]
+&gt;&gt;&gt; list(enumerate(seasons, start=1))
+[(1, 'Spring'), (2, 'Summer'), (3, 'Fall'), (4, 'Winter')]
+</t>
+  </si>
+  <si>
+    <t>11. eval(expression, globals=None, locals=None)</t>
+  </si>
+  <si>
+    <t>执行表达式expressiong, 并返回其结果，该表达式为字符串。 两个参数都必须为字典</t>
+  </si>
+  <si>
+    <t>12. exec(object[, globals[, locals]])</t>
+  </si>
+  <si>
+    <t>和eval类似，但是只返回None，也就是说只执行表达式，但是不返回结果</t>
+  </si>
+  <si>
+    <t>13. filter(function, iterable)</t>
+  </si>
+  <si>
+    <t>和(item for item in iterable if function(item))等价，itertools.filterfalse()为其互补函数</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14. frozenset([iterable]) </t>
+  </si>
+  <si>
+    <t>生成不可变集合</t>
+  </si>
+  <si>
+    <t>使用openpyxl查看和更改excel文件</t>
+  </si>
+  <si>
+    <t>from openpyxl import load_workbook
+workbook = load_workbook(filename="C:\\dtn\\XX.xlsx")  打开excel文件</t>
+  </si>
+  <si>
+    <t>或者</t>
+  </si>
+  <si>
+    <t>from openpyxl import Workbook
+workbook = Workbook() 创建excel文件</t>
+  </si>
+  <si>
+    <t>workbook.sheetnames  所有worksheet名字列表
+workbook.active 返回当前默认选中的worksheet
+workbook.get_sheet_by_name(name) 根据名称获得worksheet
+workbook.remove(worksheet) 删除worksheet对象，不是名称
+workbook.save(filename) 保存到文件，有写操作记得保存
+workbook.create_sheet() 新建worksheet
+worksheet = workbook['Sheet1'] 通过名称获取worksheet
+worksheet的属性
+rows 返回所有有效数据行，有数据时为generator，无数据时为tuple
+columns 返回所有有效数据列，类型同rows
+max_column 最大列
+max_row:有效数据最大行
+min_column:有效数据最小列,起始为1
+min_row:有效数据最大行,起始为1
+values:返回所有单元格的值的列表,类型为tuple
+title:WorkSheet的名称</t>
+  </si>
+  <si>
+    <t># 1. load module
+from openpyxl import load_workbook
+dest_filename = 'test.xlsx'
+# 2. load Workbook from existed file
+wb=load_workbook(dest_filename)
+# 3. get a WorkSheet
+ws=wb['Sheet1']
+# 4. modify data
+ws['A10']=100
+ws.cell(row=1,column=1,value=100)
+# 5. read data
+# read data
+for row in ws.rows: # 返回的row是一个tuple对象
+    for cell in row:
+        print 'row: %s  column: %s  value: %s' % (cell.row,cell.column,cell.value)
+# 6. save Workbook to file
+wb.save(dest_filename)</t>
+  </si>
+  <si>
+    <t>cell(coordinate=None, row=None, column=None, value=None): 获取指定单元格或设置单元格的值,具体使用在cell下面介绍
+# 使用WorkSheet的Cell方法
+c1=ws.cell('A1')
+c2=ws.cell(row=1,column=1) # 获取A1单元格
+# 通过坐标获取Cell
+c3=ws['A1']
+# 获取多个
+c3=ws['A1:E5'] // 返回多行数据,类型为tuple
+# 直接使用WorkSheet的cell方法设置
+ws.cell(row=1,column=1,value=10)
+# 设置Cell对象value属性
+c1=ws.cell('A1')
+c1.value=100
+column:所在列,起始为1
+row:所在行,起始为1
+coordinate: 所在坐标,如'A1'
+parent: 所属的WorkSheet
+value: 单元格的值
+offset(row=0, column=0): 偏移</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decode的作用是将其他编码的字符串转换成unicode编码，如str1.decode('gb2312')，表示将gb2312编码的字符串str1转换成unicode编码。 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">encode的作用是将unicode编码转换成其他编码的字符串，如str2.encode('gb2312')，表示将unicode编码的字符串str2转换成gb2312编码。 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     # bytes object
+      b = b"example"
+      # str object
+      s = "example"
+      # str to bytes
+      bytes(s, encoding = "utf8")
+      # bytes to str
+      str(b, encoding = "utf-8")
+      # an alternative method
+      # str to bytes
+      str.encode(s)
+      # bytes to str
+      bytes.decode(b)</t>
   </si>
 </sst>
 </file>
@@ -818,60 +1200,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="79.7109375" customWidth="1"/>
-    <col min="3" max="3" width="83.5703125" customWidth="1"/>
+    <col min="1" max="1" width="79.6640625" customWidth="1"/>
+    <col min="3" max="3" width="83.5546875" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -884,7 +1266,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
@@ -897,7 +1279,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
@@ -910,7 +1292,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -923,7 +1305,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -936,7 +1318,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>22</v>
       </c>
@@ -949,7 +1331,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>24</v>
       </c>
@@ -962,7 +1344,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>26</v>
       </c>
@@ -975,7 +1357,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
@@ -988,7 +1370,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
@@ -1001,7 +1383,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
@@ -1014,7 +1396,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>33</v>
       </c>
@@ -1027,7 +1409,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>35</v>
       </c>
@@ -1040,7 +1422,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>38</v>
       </c>
@@ -1053,7 +1435,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>41</v>
       </c>
@@ -1066,7 +1448,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>43</v>
       </c>
@@ -1079,7 +1461,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>45</v>
       </c>
@@ -1092,7 +1474,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>47</v>
       </c>
@@ -1105,7 +1487,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>49</v>
       </c>
@@ -1118,7 +1500,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>50</v>
       </c>
@@ -1131,7 +1513,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>51</v>
       </c>
@@ -1144,7 +1526,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>52</v>
       </c>
@@ -1157,72 +1539,72 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="228" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="228" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>72</v>
       </c>
@@ -1230,82 +1612,523 @@
         <v>74</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="61" spans="1:3" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A61" s="5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" ht="255" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+      <c r="C61" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C61" s="5" t="s">
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="63" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="65" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A65" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="69" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" ht="195" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
+      <c r="C69" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C69" s="5" t="s">
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="71" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A71" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
+      <c r="C71" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C71" s="5" t="s">
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A75" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A77" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A79" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A81" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A82" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A84" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A87" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A90" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A91" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A92" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A96" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A98" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" ht="288" x14ac:dyDescent="0.3">
+      <c r="A102" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="64.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="124.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="345.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E4:E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="88.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>